<commit_message>
add table in import
</commit_message>
<xml_diff>
--- a/Format-Input-APBDP.xlsx
+++ b/Format-Input-APBDP.xlsx
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>62</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="3">
-        <v>63</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="3">
-        <v>64</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="3">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="3">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="3">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,10 +664,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>14</v>
       </c>
@@ -675,7 +675,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="3">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,10 +686,10 @@
         <v>9</v>
       </c>
       <c r="C14" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -697,7 +697,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="3">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="3">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="3">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="3">
-        <v>74</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="3">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="3">
-        <v>76</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="3">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,10 +774,10 @@
         <v>17</v>
       </c>
       <c r="C22" s="3">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>24</v>
       </c>
@@ -785,7 +785,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="3">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="3">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="3">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="3">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="3">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="3">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="3">
-        <v>85</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>25</v>
       </c>
       <c r="C30" s="3">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="3">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,7 +884,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="3">
-        <v>88</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="3">
-        <v>89</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="3">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,7 +917,7 @@
         <v>30</v>
       </c>
       <c r="C35" s="3">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,7 +928,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="3">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
         <v>32</v>
       </c>
       <c r="C37" s="3">
-        <v>93</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -950,7 +950,7 @@
         <v>33</v>
       </c>
       <c r="C38" s="3">
-        <v>94</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>34</v>
       </c>
       <c r="C39" s="3">
-        <v>95</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -972,7 +972,7 @@
         <v>35</v>
       </c>
       <c r="C40" s="3">
-        <v>96</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
         <v>36</v>
       </c>
       <c r="C41" s="3">
-        <v>97</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -994,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="C42" s="3">
-        <v>98</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,7 +1005,7 @@
         <v>38</v>
       </c>
       <c r="C43" s="3">
-        <v>99</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,7 +1016,7 @@
         <v>39</v>
       </c>
       <c r="C44" s="3">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,7 +1027,7 @@
         <v>40</v>
       </c>
       <c r="C45" s="3">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>41</v>
       </c>
       <c r="C46" s="3">
-        <v>102</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>